<commit_message>
Added Description for Cost
</commit_message>
<xml_diff>
--- a/Documents/OpenRead Timeline.xlsx
+++ b/Documents/OpenRead Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Steven/Desktop/SRS Everything/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151DEF18-901D-3446-8951-E0A627B4ABAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E485E17-B875-8B49-97D4-A3C11B956565}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{4C8EC219-729B-5A4D-AF0F-DF2374F91EB9}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
   <si>
     <t>LA06</t>
   </si>
@@ -257,6 +257,69 @@
   </si>
   <si>
     <t>Others</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Total Electricity Cost</t>
+  </si>
+  <si>
+    <t>Internet Cost</t>
+  </si>
+  <si>
+    <t>Planning, overseeing, and leading the whole process of the projects</t>
+  </si>
+  <si>
+    <t>Design the interfaces for the application</t>
+  </si>
+  <si>
+    <t>Laptops that are required for the project</t>
+  </si>
+  <si>
+    <t>Backend Developer (Responsible for the server-side logic)</t>
+  </si>
+  <si>
+    <t>Frontend Developer (Responsible for converting data into a graphical interface)</t>
+  </si>
+  <si>
+    <t>Implement Programs and Ensure fit to user needs</t>
+  </si>
+  <si>
+    <t>Human Resource</t>
+  </si>
+  <si>
+    <t>Visual Studio Code</t>
+  </si>
+  <si>
+    <t>For Frontend Development</t>
+  </si>
+  <si>
+    <t>Microsoft Office</t>
+  </si>
+  <si>
+    <t>For Documents (Word and Excel)</t>
+  </si>
+  <si>
+    <t>mySQL</t>
+  </si>
+  <si>
+    <t>Programming Language for web development</t>
+  </si>
+  <si>
+    <t>Database Management System for database needed for storing user credentials and story</t>
+  </si>
+  <si>
+    <t>Photoshop</t>
+  </si>
+  <si>
+    <t>Adobe Photoshop needed for graphical design (1 month)</t>
+  </si>
+  <si>
+    <t>Software Tester to conduct tests to ensure the quality of the web-application</t>
+  </si>
+  <si>
+    <t>php</t>
   </si>
 </sst>
 </file>
@@ -264,7 +327,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="\R\p\ ###0.00;[Red]&quot;IDR&quot;###0.00"/>
+    <numFmt numFmtId="164" formatCode="\R\p\ ###0.00;[Red]&quot;IDR&quot;###0.00"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -345,7 +408,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +463,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -645,7 +720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -690,54 +765,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -750,27 +777,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -794,8 +800,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -803,7 +809,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -812,7 +818,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -822,56 +827,149 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1204,48 +1302,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="20"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="55"/>
     </row>
     <row r="2" spans="1:22" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="23"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="58"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -1268,15 +1366,15 @@
       <c r="S3" s="1"/>
     </row>
     <row r="4" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="72"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1474,51 +1572,51 @@
       <c r="V13" s="13"/>
     </row>
     <row r="14" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="26"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="60"/>
+      <c r="R14" s="60"/>
+      <c r="S14" s="61"/>
       <c r="T14" s="14"/>
       <c r="U14" s="13"/>
       <c r="V14" s="13"/>
     </row>
     <row r="15" spans="1:22" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="29"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="64"/>
       <c r="T15" s="14"/>
       <c r="U15" s="13"/>
       <c r="V15" s="13"/>
@@ -1552,95 +1650,95 @@
       <c r="V17" s="13"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="41"/>
-      <c r="F18" s="42" t="s">
+      <c r="E18" s="51"/>
+      <c r="F18" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42" t="s">
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="42" t="s">
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="41" t="s">
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="S18" s="43"/>
+      <c r="S18" s="52"/>
       <c r="T18" s="13"/>
       <c r="U18" s="13"/>
       <c r="V18" s="13"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A19" s="44"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="46">
+      <c r="A19" s="66"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="23">
         <v>3</v>
       </c>
-      <c r="E19" s="46">
+      <c r="E19" s="23">
         <v>4</v>
       </c>
-      <c r="F19" s="46">
+      <c r="F19" s="23">
         <v>1</v>
       </c>
-      <c r="G19" s="46">
+      <c r="G19" s="23">
         <v>2</v>
       </c>
-      <c r="H19" s="46">
+      <c r="H19" s="23">
         <v>3</v>
       </c>
-      <c r="I19" s="46">
+      <c r="I19" s="23">
         <v>4</v>
       </c>
-      <c r="J19" s="46">
+      <c r="J19" s="23">
         <v>1</v>
       </c>
-      <c r="K19" s="46">
+      <c r="K19" s="23">
         <v>2</v>
       </c>
-      <c r="L19" s="46">
+      <c r="L19" s="23">
         <v>3</v>
       </c>
-      <c r="M19" s="46">
+      <c r="M19" s="23">
         <v>4</v>
       </c>
-      <c r="N19" s="46">
+      <c r="N19" s="23">
         <v>1</v>
       </c>
-      <c r="O19" s="46">
+      <c r="O19" s="23">
         <v>2</v>
       </c>
-      <c r="P19" s="46">
+      <c r="P19" s="23">
         <v>3</v>
       </c>
-      <c r="Q19" s="46">
+      <c r="Q19" s="23">
         <v>4</v>
       </c>
-      <c r="R19" s="47">
+      <c r="R19" s="24">
         <v>1</v>
       </c>
-      <c r="S19" s="48">
+      <c r="S19" s="25">
         <v>2</v>
       </c>
       <c r="T19" s="13"/>
@@ -1648,13 +1746,13 @@
       <c r="V19" s="13"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="15"/>
@@ -1676,17 +1774,17 @@
       <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
-      <c r="S20" s="35"/>
+      <c r="S20" s="19"/>
       <c r="T20" s="13"/>
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
-      <c r="B21" s="34" t="s">
+      <c r="A21" s="26"/>
+      <c r="B21" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="15"/>
@@ -1706,14 +1804,14 @@
       <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
-      <c r="S21" s="35"/>
+      <c r="S21" s="19"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="49"/>
-      <c r="B22" s="34" t="s">
+      <c r="A22" s="26"/>
+      <c r="B22" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="15"/>
@@ -1743,16 +1841,16 @@
       <c r="P22" s="15"/>
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
-      <c r="S22" s="35"/>
+      <c r="S22" s="19"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A23" s="49" t="s">
+      <c r="A23" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D23" s="15"/>
@@ -1774,14 +1872,14 @@
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
-      <c r="S23" s="35"/>
+      <c r="S23" s="19"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" s="49"/>
-      <c r="B24" s="34" t="s">
+      <c r="A24" s="26"/>
+      <c r="B24" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="15"/>
@@ -1803,16 +1901,16 @@
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
-      <c r="S24" s="35"/>
+      <c r="S24" s="19"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="15"/>
@@ -1836,16 +1934,16 @@
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
-      <c r="S25" s="35"/>
+      <c r="S25" s="19"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="18" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="15"/>
@@ -1865,14 +1963,14 @@
       </c>
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
-      <c r="S26" s="35"/>
+      <c r="S26" s="19"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A27" s="49"/>
-      <c r="B27" s="34" t="s">
+      <c r="A27" s="26"/>
+      <c r="B27" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="18" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="15"/>
@@ -1890,18 +1988,18 @@
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
-      <c r="S27" s="35" t="s">
+      <c r="S27" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="18" t="s">
         <v>44</v>
       </c>
       <c r="D28" s="15"/>
@@ -1923,14 +2021,14 @@
         <v>30</v>
       </c>
       <c r="R28" s="15"/>
-      <c r="S28" s="35"/>
+      <c r="S28" s="19"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="50"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="18" t="s">
         <v>44</v>
       </c>
       <c r="D29" s="13"/>
@@ -1950,14 +2048,14 @@
         <v>30</v>
       </c>
       <c r="R29" s="15"/>
-      <c r="S29" s="35"/>
+      <c r="S29" s="19"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A30" s="50"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="18" t="s">
         <v>44</v>
       </c>
       <c r="D30" s="13"/>
@@ -1979,14 +2077,14 @@
       <c r="R30" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="S30" s="35"/>
+      <c r="S30" s="19"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A31" s="50"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="18" t="s">
         <v>44</v>
       </c>
       <c r="D31" s="13"/>
@@ -2008,34 +2106,34 @@
       <c r="R31" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="S31" s="35"/>
+      <c r="S31" s="19"/>
     </row>
     <row r="32" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="36"/>
-      <c r="P32" s="37"/>
-      <c r="Q32" s="37"/>
-      <c r="R32" s="37"/>
-      <c r="S32" s="38" t="s">
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2060,345 +2158,491 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C12DA1-FD1E-9D48-8B4B-48E074C87B35}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="70"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="71"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="73"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="52"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="54"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="62" t="s">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="75"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="76"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="78"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="31"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="E4" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="65" t="s">
+      <c r="F4" s="90"/>
+      <c r="G4" s="41" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="66" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="55">
+      <c r="C5" s="89" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="32">
         <v>4</v>
       </c>
-      <c r="D5" s="56">
+      <c r="E5" s="33">
         <v>10000000</v>
       </c>
-      <c r="E5" s="55"/>
-      <c r="F5" s="57">
-        <f>C5*D5</f>
+      <c r="F5" s="90"/>
+      <c r="G5" s="34">
+        <f>D5*E5</f>
         <v>40000000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="67" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="90"/>
+      <c r="G6" s="34">
+        <f>D6*E6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="93"/>
+      <c r="B7" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="89" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="90"/>
+      <c r="G7" s="34">
+        <f t="shared" ref="G7:G10" si="0">D7*E7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="93"/>
+      <c r="B8" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="90"/>
+      <c r="G8" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="93"/>
+      <c r="B9" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="89" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="32">
+        <v>1</v>
+      </c>
+      <c r="E9" s="33">
+        <v>150000</v>
+      </c>
+      <c r="F9" s="90"/>
+      <c r="G9" s="34">
+        <f t="shared" si="0"/>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="93"/>
+      <c r="B10" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="89" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="32">
+        <v>1</v>
+      </c>
+      <c r="E10" s="33">
+        <v>350000</v>
+      </c>
+      <c r="F10" s="90"/>
+      <c r="G10" s="34">
+        <f t="shared" si="0"/>
+        <v>350000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="55">
+      <c r="C11" s="89" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="32">
         <v>1</v>
       </c>
-      <c r="D6" s="56">
+      <c r="E11" s="33">
         <v>100000000</v>
       </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="57">
-        <f t="shared" ref="F6:F11" si="0">C6*D6</f>
+      <c r="F11" s="90"/>
+      <c r="G11" s="34">
+        <f>D11*E11</f>
         <v>100000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
-      <c r="B7" s="55" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="29"/>
+      <c r="B12" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="55">
+      <c r="C12" s="89" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="32">
         <v>1</v>
       </c>
-      <c r="D7" s="56">
+      <c r="E12" s="33">
         <v>5000000</v>
       </c>
-      <c r="E7" s="53"/>
-      <c r="F7" s="57">
-        <f t="shared" si="0"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="34">
+        <f>D12*E12</f>
         <v>5000000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
-      <c r="B8" s="55" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="29"/>
+      <c r="B13" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="55">
+      <c r="C13" s="89" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="32">
         <v>1</v>
       </c>
-      <c r="D8" s="56">
+      <c r="E13" s="33">
         <v>20000000</v>
       </c>
-      <c r="E8" s="53"/>
-      <c r="F8" s="57">
-        <f t="shared" si="0"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="34">
+        <f>D13*E13</f>
         <v>20000000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
-      <c r="B9" s="55" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="29"/>
+      <c r="B14" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="55">
+      <c r="C14" s="89" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="32">
         <v>2</v>
       </c>
-      <c r="D9" s="56">
+      <c r="E14" s="33">
         <v>10000000</v>
       </c>
-      <c r="E9" s="53"/>
-      <c r="F9" s="57">
-        <f t="shared" si="0"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="34">
+        <f>D14*E14</f>
         <v>20000000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
-      <c r="B10" s="55" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="29"/>
+      <c r="B15" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="55">
+      <c r="C15" s="89" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="32">
         <v>1</v>
       </c>
-      <c r="D10" s="56">
+      <c r="E15" s="33">
         <v>10000000</v>
       </c>
-      <c r="E10" s="53"/>
-      <c r="F10" s="57">
-        <f t="shared" si="0"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="34">
+        <f>D15*E15</f>
         <v>10000000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="52"/>
-      <c r="B11" s="55" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="29"/>
+      <c r="B16" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="55">
+      <c r="C16" s="89" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="32">
         <v>1</v>
       </c>
-      <c r="D11" s="56">
+      <c r="E16" s="33">
         <v>3000000</v>
       </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="57">
-        <f t="shared" si="0"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="34">
+        <f>D16*E16</f>
         <v>3000000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="52"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="58"/>
-    </row>
-    <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="35"/>
+    </row>
+    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="61">
-        <f>SUM(F5:F11)</f>
-        <v>198000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="74" t="s">
+      <c r="G18" s="38">
+        <f>SUM(G5:G16)</f>
+        <v>198500000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="78"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="76"/>
-      <c r="B16" s="77"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="79"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="62" t="s">
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="81"/>
+    </row>
+    <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="82"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="84"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B22" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C22" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="54"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="80" t="s">
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="31"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="81" t="s">
+      <c r="B23" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="82">
+      <c r="C23" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="45">
         <v>5000000</v>
       </c>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="54"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="80"/>
-      <c r="B19" s="81" t="s">
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="31"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="91"/>
+      <c r="B24" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="82">
+      <c r="C24" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="45">
         <v>2000000</v>
       </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="54"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="80" t="s">
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="31"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="83"/>
-      <c r="C20" s="82">
-        <f>F13</f>
-        <v>198000000</v>
-      </c>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="54"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="80" t="s">
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="45">
+        <f>G18</f>
+        <v>198500000</v>
+      </c>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="31"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B26" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="82">
+      <c r="C26" s="30"/>
+      <c r="D26" s="45">
         <v>500000</v>
       </c>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="54"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="80" t="s">
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="31"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="53"/>
-      <c r="C22" s="82">
-        <f>0.1*SUM(C18:C21)</f>
-        <v>20550000</v>
-      </c>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="54"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="80" t="s">
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="45">
+        <f>0.1*SUM(D23:D26)</f>
+        <v>20600000</v>
+      </c>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="31"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="82">
-        <f>0.3*SUM(C18:C22)</f>
-        <v>67815000</v>
-      </c>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="54"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="54"/>
-    </row>
-    <row r="25" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-      <c r="B25" s="85" t="s">
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="45">
+        <f>0.3*SUM(D23:D27)</f>
+        <v>67980000</v>
+      </c>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="31"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="29"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="31"/>
+    </row>
+    <row r="30" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="36"/>
+      <c r="B30" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="86">
-        <f>SUM(C18:C23)</f>
-        <v>293865000</v>
-      </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="84"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="49">
+        <f>SUM(D23:D28)</f>
+        <v>294580000</v>
+      </c>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A15:F16"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A20:G21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="F3:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>